<commit_message>
Fan Motor control Logic Documentation Updated
</commit_message>
<xml_diff>
--- a/Delivery Process Documentation.xlsx
+++ b/Delivery Process Documentation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OVEN_Project\19-08-2023\Oven_Documentations\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OVEN_Project\19-08-2023\Oven_Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -446,7 +446,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -506,33 +506,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,12 +550,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -580,27 +559,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -612,6 +585,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -896,14 +884,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26" style="8" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="5" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" customWidth="1"/>
     <col min="5" max="5" width="31.36328125" customWidth="1"/>
     <col min="6" max="6" width="18.81640625" customWidth="1"/>
@@ -912,289 +898,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="28">
+      <c r="A5" s="22">
         <v>2</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="14" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="6" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="26"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="6" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="26"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="26"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="13" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
+      <c r="A13" s="9">
         <v>4</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="18"/>
+      <c r="E13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="28" t="s">
         <v>19</v>
       </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E14" s="7"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7">
+      <c r="A15" s="9">
         <v>5</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="18">
         <v>3</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="23" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D18" s="27"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+      <c r="A19" s="17">
         <v>4</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D20" s="27"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="A21" s="17">
         <v>5</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="23" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+      <c r="A23" s="5">
         <v>6</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="16"/>
+      <c r="E23" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="116" x14ac:dyDescent="0.35">
-      <c r="A25" s="7">
+      <c r="A25" s="5">
         <v>7</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E26" s="12"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="7">
+      <c r="A27" s="5">
         <v>8</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F27" t="s">
@@ -1202,13 +1206,13 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="7">
+      <c r="A29" s="5">
         <v>9</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F29" t="s">
@@ -1216,22 +1220,22 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="391.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="7">
+      <c r="A31" s="5">
         <v>10</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="H31" s="11" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Component list Document added
</commit_message>
<xml_diff>
--- a/Delivery Process Documentation.xlsx
+++ b/Delivery Process Documentation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>SL</t>
   </si>
@@ -395,6 +395,45 @@
       <t xml:space="preserve"> 
 &gt;if any issues during the BLE Module configurations Refer the HC-05 Data sheet and Bluetooth Configuration document.</t>
     </r>
+  </si>
+  <si>
+    <t>Class D Audio Board &amp; Speaker</t>
+  </si>
+  <si>
+    <t>Speaker Wire</t>
+  </si>
+  <si>
+    <t>Audio jack (Refer the sample)</t>
+  </si>
+  <si>
+    <t>Cable conn</t>
+  </si>
+  <si>
+    <t>Ravi Electronics</t>
+  </si>
+  <si>
+    <t>Single socket Switch box</t>
+  </si>
+  <si>
+    <t>Bolt &amp; nuts</t>
+  </si>
+  <si>
+    <t>Pandian store</t>
+  </si>
+  <si>
+    <t>Any electrical shop</t>
+  </si>
+  <si>
+    <t>Any mobile shop</t>
+  </si>
+  <si>
+    <t>&gt;Used for Connect the Tablet charger this switch board is connected with the 8th relay</t>
+  </si>
+  <si>
+    <t>&gt;Refere sample audio jack, the audio jack head should be smaller</t>
+  </si>
+  <si>
+    <t>&gt;54 inch wire is needed for one speaker .</t>
   </si>
 </sst>
 </file>
@@ -565,6 +604,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -572,6 +620,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -585,21 +639,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -882,9 +921,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -941,22 +982,22 @@
       <c r="G3" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="22">
+      <c r="A5" s="27">
         <v>2</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="28" t="s">
         <v>27</v>
       </c>
       <c r="G5" s="12" t="s">
@@ -965,70 +1006,70 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="20" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="13" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>4</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -1038,7 +1079,7 @@
       <c r="E13" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="20" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="4"/>
@@ -1061,13 +1102,13 @@
       <c r="E15" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1078,8 +1119,8 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
@@ -1089,25 +1130,25 @@
         <v>23</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="30" t="s">
+      <c r="D17" s="26"/>
+      <c r="E17" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="17">
@@ -1117,21 +1158,21 @@
         <v>24</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="17">
@@ -1141,11 +1182,11 @@
         <v>25</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="23" spans="1:8" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
@@ -1161,16 +1202,16 @@
       <c r="F23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" spans="1:8" ht="116" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
@@ -1185,8 +1226,8 @@
       <c r="F25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E26" s="10"/>
@@ -1237,6 +1278,85 @@
       </c>
       <c r="H31" s="11" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+      <c r="H39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>